<commit_message>
Update check for start lesson when user import edit
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_StudentNumberValid.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_StudentNumberValid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F972E37-939D-49AC-AA50-FE3CCE7FA965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F68AEA1-C0DD-4B92-A8B6-F070437F9D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9587" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9665" uniqueCount="864">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -5435,7 +5435,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5572,6 +5572,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5945,7 +5951,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5990,9 +5996,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -6353,10 +6356,10 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="R56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA9" sqref="AA9"/>
+      <selection pane="bottomRight" activeCell="AA79" sqref="AA79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6554,8 +6557,8 @@
       <c r="Y2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" s="19">
-        <v>1</v>
+      <c r="Z2" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA2" s="6" t="s">
         <v>50</v>
@@ -6650,8 +6653,8 @@
       <c r="Y3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z3" s="19">
-        <v>1</v>
+      <c r="Z3" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA3" s="8" t="s">
         <v>66</v>
@@ -6746,8 +6749,8 @@
       <c r="Y4" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z4" s="19">
-        <v>1</v>
+      <c r="Z4" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA4" s="8" t="s">
         <v>66</v>
@@ -6843,7 +6846,7 @@
         <v>50</v>
       </c>
       <c r="Z5" s="19" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="AA5" s="8" t="s">
         <v>66</v>
@@ -6936,8 +6939,8 @@
       <c r="Y6" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z6" s="19">
-        <v>1</v>
+      <c r="Z6" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA6" s="8" t="s">
         <v>50</v>
@@ -7032,8 +7035,8 @@
       <c r="Y7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z7" s="19">
-        <v>1</v>
+      <c r="Z7" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA7" s="8" t="s">
         <v>66</v>
@@ -7128,8 +7131,8 @@
       <c r="Y8" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z8" s="19">
-        <v>1</v>
+      <c r="Z8" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA8" s="8" t="s">
         <v>66</v>
@@ -7225,7 +7228,7 @@
         <v>89</v>
       </c>
       <c r="Z9" s="19" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="AA9" s="8" t="s">
         <v>66</v>
@@ -7320,8 +7323,8 @@
       <c r="Y10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z10" s="19">
-        <v>1</v>
+      <c r="Z10" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA10" s="8" t="s">
         <v>50</v>
@@ -7416,8 +7419,8 @@
       <c r="Y11" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z11" s="19">
-        <v>1</v>
+      <c r="Z11" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA11" s="8" t="s">
         <v>66</v>
@@ -7512,8 +7515,8 @@
       <c r="Y12" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z12" s="19">
-        <v>1</v>
+      <c r="Z12" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA12" s="8" t="s">
         <v>66</v>
@@ -7608,8 +7611,8 @@
       <c r="Y13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z13" s="20">
-        <v>1</v>
+      <c r="Z13" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA13" s="8" t="s">
         <v>66</v>
@@ -7704,8 +7707,8 @@
       <c r="Y14" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z14" s="20">
-        <v>1</v>
+      <c r="Z14" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA14" s="8" t="s">
         <v>50</v>
@@ -7800,8 +7803,8 @@
       <c r="Y15" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z15" s="20">
-        <v>1</v>
+      <c r="Z15" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA15" s="8" t="s">
         <v>66</v>
@@ -7896,8 +7899,8 @@
       <c r="Y16" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z16" s="20">
-        <v>1</v>
+      <c r="Z16" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA16" s="8" t="s">
         <v>66</v>
@@ -7992,8 +7995,8 @@
       <c r="Y17" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z17" s="20">
-        <v>1</v>
+      <c r="Z17" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA17" s="8" t="s">
         <v>66</v>
@@ -8088,8 +8091,8 @@
       <c r="Y18" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z18" s="20">
-        <v>1</v>
+      <c r="Z18" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA18" s="8" t="s">
         <v>50</v>
@@ -8184,8 +8187,8 @@
       <c r="Y19" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z19" s="20">
-        <v>1</v>
+      <c r="Z19" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA19" s="8" t="s">
         <v>66</v>
@@ -8278,8 +8281,8 @@
       <c r="Y20" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z20" s="20">
-        <v>1</v>
+      <c r="Z20" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA20" s="8" t="s">
         <v>66</v>
@@ -8374,8 +8377,8 @@
       <c r="Y21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z21" s="20">
-        <v>1</v>
+      <c r="Z21" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA21" s="8" t="s">
         <v>66</v>
@@ -8470,8 +8473,8 @@
       <c r="Y22" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z22" s="20">
-        <v>1</v>
+      <c r="Z22" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA22" s="8" t="s">
         <v>50</v>
@@ -8566,8 +8569,8 @@
       <c r="Y23" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z23" s="20">
-        <v>1</v>
+      <c r="Z23" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA23" s="8" t="s">
         <v>66</v>
@@ -8662,8 +8665,8 @@
       <c r="Y24" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z24" s="20">
-        <v>1</v>
+      <c r="Z24" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA24" s="8" t="s">
         <v>66</v>
@@ -8758,8 +8761,8 @@
       <c r="Y25" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z25" s="20">
-        <v>1</v>
+      <c r="Z25" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA25" s="8" t="s">
         <v>66</v>
@@ -8852,8 +8855,8 @@
       <c r="Y26" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z26" s="20">
-        <v>1</v>
+      <c r="Z26" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA26" s="8" t="s">
         <v>50</v>
@@ -8948,8 +8951,8 @@
       <c r="Y27" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z27" s="20">
-        <v>1</v>
+      <c r="Z27" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA27" s="8" t="s">
         <v>66</v>
@@ -9044,8 +9047,8 @@
       <c r="Y28" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z28" s="20">
-        <v>1</v>
+      <c r="Z28" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA28" s="8" t="s">
         <v>66</v>
@@ -9140,8 +9143,8 @@
       <c r="Y29" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z29" s="20">
-        <v>1</v>
+      <c r="Z29" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA29" s="8" t="s">
         <v>66</v>
@@ -9236,8 +9239,8 @@
       <c r="Y30" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z30" s="20">
-        <v>1</v>
+      <c r="Z30" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA30" s="8" t="s">
         <v>50</v>
@@ -9332,8 +9335,8 @@
       <c r="Y31" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z31" s="20">
-        <v>1</v>
+      <c r="Z31" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA31" s="8" t="s">
         <v>66</v>
@@ -9428,8 +9431,8 @@
       <c r="Y32" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="Z32" s="20">
-        <v>1</v>
+      <c r="Z32" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA32" s="6" t="s">
         <v>66</v>
@@ -9526,8 +9529,8 @@
       <c r="Y33" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z33" s="20">
-        <v>1</v>
+      <c r="Z33" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA33" s="8" t="s">
         <v>66</v>
@@ -9622,8 +9625,8 @@
       <c r="Y34" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z34" s="20">
-        <v>1</v>
+      <c r="Z34" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA34" s="8" t="s">
         <v>50</v>
@@ -9718,8 +9721,8 @@
       <c r="Y35" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z35" s="20">
-        <v>1</v>
+      <c r="Z35" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA35" s="8" t="s">
         <v>66</v>
@@ -9814,8 +9817,8 @@
       <c r="Y36" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z36" s="20">
-        <v>1</v>
+      <c r="Z36" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA36" s="8" t="s">
         <v>66</v>
@@ -9910,8 +9913,8 @@
       <c r="Y37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z37" s="20">
-        <v>1</v>
+      <c r="Z37" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA37" s="8" t="s">
         <v>66</v>
@@ -10006,8 +10009,8 @@
       <c r="Y38" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z38" s="20">
-        <v>1</v>
+      <c r="Z38" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA38" s="8" t="s">
         <v>50</v>
@@ -10102,8 +10105,8 @@
       <c r="Y39" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z39" s="20">
-        <v>1</v>
+      <c r="Z39" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA39" s="8" t="s">
         <v>66</v>
@@ -10198,8 +10201,8 @@
       <c r="Y40" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z40" s="20">
-        <v>1</v>
+      <c r="Z40" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA40" s="8" t="s">
         <v>66</v>
@@ -10294,8 +10297,8 @@
       <c r="Y41" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z41" s="20">
-        <v>1</v>
+      <c r="Z41" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA41" s="8" t="s">
         <v>66</v>
@@ -10386,8 +10389,8 @@
       <c r="Y42" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z42" s="20">
-        <v>1</v>
+      <c r="Z42" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA42" s="8" t="s">
         <v>50</v>
@@ -10482,8 +10485,8 @@
       <c r="Y43" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z43" s="20">
-        <v>1</v>
+      <c r="Z43" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA43" s="8" t="s">
         <v>66</v>
@@ -10578,8 +10581,8 @@
       <c r="Y44" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z44" s="20">
-        <v>1</v>
+      <c r="Z44" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA44" s="8" t="s">
         <v>66</v>
@@ -10674,8 +10677,8 @@
       <c r="Y45" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z45" s="20">
-        <v>1</v>
+      <c r="Z45" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA45" s="8" t="s">
         <v>66</v>
@@ -10766,8 +10769,8 @@
       <c r="Y46" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z46" s="20">
-        <v>1</v>
+      <c r="Z46" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA46" s="8" t="s">
         <v>50</v>
@@ -10860,8 +10863,8 @@
       <c r="Y47" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z47" s="20">
-        <v>1</v>
+      <c r="Z47" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA47" s="8" t="s">
         <v>66</v>
@@ -10956,8 +10959,8 @@
       <c r="Y48" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z48" s="20">
-        <v>1</v>
+      <c r="Z48" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA48" s="8" t="s">
         <v>66</v>
@@ -11052,8 +11055,8 @@
       <c r="Y49" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z49" s="20">
-        <v>1</v>
+      <c r="Z49" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA49" s="8" t="s">
         <v>66</v>
@@ -11148,8 +11151,8 @@
       <c r="Y50" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z50" s="20">
-        <v>1</v>
+      <c r="Z50" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA50" s="8" t="s">
         <v>50</v>
@@ -11244,8 +11247,8 @@
       <c r="Y51" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z51" s="20">
-        <v>1</v>
+      <c r="Z51" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA51" s="8" t="s">
         <v>66</v>
@@ -11340,8 +11343,8 @@
       <c r="Y52" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z52" s="20">
-        <v>1</v>
+      <c r="Z52" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA52" s="8" t="s">
         <v>66</v>
@@ -11436,8 +11439,8 @@
       <c r="Y53" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z53" s="20">
-        <v>1</v>
+      <c r="Z53" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA53" s="8" t="s">
         <v>66</v>
@@ -11532,8 +11535,8 @@
       <c r="Y54" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z54" s="20">
-        <v>1</v>
+      <c r="Z54" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA54" s="8" t="s">
         <v>50</v>
@@ -11628,8 +11631,8 @@
       <c r="Y55" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z55" s="20">
-        <v>1</v>
+      <c r="Z55" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA55" s="8" t="s">
         <v>66</v>
@@ -11724,8 +11727,8 @@
       <c r="Y56" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z56" s="20">
-        <v>1</v>
+      <c r="Z56" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA56" s="8" t="s">
         <v>66</v>
@@ -11820,8 +11823,8 @@
       <c r="Y57" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z57" s="20">
-        <v>1</v>
+      <c r="Z57" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA57" s="8" t="s">
         <v>66</v>
@@ -11916,8 +11919,8 @@
       <c r="Y58" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z58" s="20">
-        <v>1</v>
+      <c r="Z58" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA58" s="8" t="s">
         <v>50</v>
@@ -12012,8 +12015,8 @@
       <c r="Y59" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z59" s="20">
-        <v>1</v>
+      <c r="Z59" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA59" s="8" t="s">
         <v>66</v>
@@ -12108,8 +12111,8 @@
       <c r="Y60" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z60" s="20">
-        <v>1</v>
+      <c r="Z60" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA60" s="8" t="s">
         <v>66</v>
@@ -12204,8 +12207,8 @@
       <c r="Y61" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z61" s="20">
-        <v>1</v>
+      <c r="Z61" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA61" s="8" t="s">
         <v>66</v>
@@ -12300,8 +12303,8 @@
       <c r="Y62" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z62" s="20">
-        <v>1</v>
+      <c r="Z62" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA62" s="8" t="s">
         <v>50</v>
@@ -12396,8 +12399,8 @@
       <c r="Y63" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z63" s="20">
-        <v>1</v>
+      <c r="Z63" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA63" s="8" t="s">
         <v>66</v>
@@ -12492,8 +12495,8 @@
       <c r="Y64" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z64" s="20">
-        <v>1</v>
+      <c r="Z64" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA64" s="8" t="s">
         <v>66</v>
@@ -12588,8 +12591,8 @@
       <c r="Y65" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z65" s="20">
-        <v>1</v>
+      <c r="Z65" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA65" s="8" t="s">
         <v>66</v>
@@ -12684,8 +12687,8 @@
       <c r="Y66" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z66" s="20">
-        <v>1</v>
+      <c r="Z66" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA66" s="8" t="s">
         <v>50</v>
@@ -12780,8 +12783,8 @@
       <c r="Y67" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z67" s="20">
-        <v>1</v>
+      <c r="Z67" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA67" s="8" t="s">
         <v>66</v>
@@ -12876,8 +12879,8 @@
       <c r="Y68" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z68" s="20">
-        <v>1</v>
+      <c r="Z68" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA68" s="8" t="s">
         <v>66</v>
@@ -12972,8 +12975,8 @@
       <c r="Y69" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z69" s="20">
-        <v>1</v>
+      <c r="Z69" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA69" s="8" t="s">
         <v>66</v>
@@ -13068,8 +13071,8 @@
       <c r="Y70" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z70" s="20">
-        <v>1</v>
+      <c r="Z70" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA70" s="8" t="s">
         <v>50</v>
@@ -13164,8 +13167,8 @@
       <c r="Y71" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z71" s="20">
-        <v>1</v>
+      <c r="Z71" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA71" s="8" t="s">
         <v>66</v>
@@ -13260,8 +13263,8 @@
       <c r="Y72" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z72" s="20">
-        <v>1</v>
+      <c r="Z72" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA72" s="8" t="s">
         <v>66</v>
@@ -13356,8 +13359,8 @@
       <c r="Y73" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z73" s="20">
-        <v>1</v>
+      <c r="Z73" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA73" s="8" t="s">
         <v>66</v>
@@ -13452,8 +13455,8 @@
       <c r="Y74" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z74" s="20">
-        <v>1</v>
+      <c r="Z74" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA74" s="8" t="s">
         <v>50</v>
@@ -13548,8 +13551,8 @@
       <c r="Y75" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z75" s="20">
-        <v>1</v>
+      <c r="Z75" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA75" s="8" t="s">
         <v>66</v>
@@ -13644,8 +13647,8 @@
       <c r="Y76" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Z76" s="20">
-        <v>1</v>
+      <c r="Z76" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA76" s="8" t="s">
         <v>66</v>
@@ -13740,8 +13743,8 @@
       <c r="Y77" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z77" s="20">
-        <v>1</v>
+      <c r="Z77" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA77" s="8" t="s">
         <v>66</v>
@@ -13836,8 +13839,8 @@
       <c r="Y78" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z78" s="20">
-        <v>1</v>
+      <c r="Z78" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA78" s="8" t="s">
         <v>50</v>
@@ -13932,8 +13935,8 @@
       <c r="Y79" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z79" s="20">
-        <v>1</v>
+      <c r="Z79" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA79" s="8" t="s">
         <v>66</v>
@@ -14028,8 +14031,8 @@
       <c r="Y80" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Z80" s="20">
-        <v>1</v>
+      <c r="Z80" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA80" s="8" t="s">
         <v>66</v>
@@ -14124,8 +14127,8 @@
       <c r="Y81" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z81" s="20">
-        <v>1</v>
+      <c r="Z81" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="AA81" s="8" t="s">
         <v>66</v>
@@ -14220,7 +14223,7 @@
       <c r="Y82" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="Z82" s="8" t="s">
+      <c r="Z82" s="19" t="s">
         <v>277</v>
       </c>
       <c r="AA82" s="8" t="s">
@@ -36322,6 +36325,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AF312" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>